<commit_message>
Added PCA to XLSX
</commit_message>
<xml_diff>
--- a/CompressionResults.xlsx
+++ b/CompressionResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maiscj\Documents\MLProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\oskar\Utvecklare\EPFL\MATH-412-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B868A5A-ED73-4B91-A083-D088A3A23965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F92EBAC-F779-4C10-A27E-79D9B9848720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{94E73D12-A8F7-4F8E-8E36-EEC12DDFF800}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94E73D12-A8F7-4F8E-8E36-EEC12DDFF800}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>Latent Size</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>JPEG2000</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>Component count</t>
+  </si>
+  <si>
+    <t>MSE</t>
   </si>
 </sst>
 </file>
@@ -102,13 +111,13 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,7 +135,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -188,7 +197,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -538,6 +547,145 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>PCA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AB$3:$AB$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AC$3:$AC$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5.4293000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5301000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7762999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1025E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4815E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9449999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4952999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1183999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1150000000000007E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.6670000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7680000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3210000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2570000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.13E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-303B-41B7-8E7D-03DA8C51F228}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -554,6 +702,7 @@
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -622,7 +771,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -660,7 +809,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="694359311"/>
@@ -671,6 +820,7 @@
         <c:axId val="694359311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.0000000000000004E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -739,7 +889,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -777,7 +927,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="694354031"/>
@@ -819,7 +969,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -849,7 +999,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="sv-SE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -863,7 +1013,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -925,7 +1075,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1399,6 +1549,145 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FD8B-4EEA-967D-81DCE6EF54B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>PCA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AB$3:$AB$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AD$3:$AD$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.29202899999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30060100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30715399999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31353500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32470500000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34683000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38312200000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43704999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.50856400000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59536900000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68652500000000005</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.77143700000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84755199999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91810999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-00F1-4B63-8E36-91D0F859D8D2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1486,7 +1775,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1524,7 +1813,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="911667215"/>
@@ -1603,7 +1892,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1641,7 +1930,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="911669615"/>
@@ -1683,7 +1972,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1713,7 +2002,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="sv-SE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1727,7 +2016,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="sv-SE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1789,7 +2078,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2263,6 +2552,145 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-85A7-48A5-B10D-413D123885F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>PCA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AB$3:$AB$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$AE$3:$AE$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>13.234030000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.017124000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.83764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.698760999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.671994000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.749154999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.925094999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.223462999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.655605999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.256789999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.073186</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.225166999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.940572</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>33.897015000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E72B-416F-B79A-89ACA3EE617D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2350,7 +2778,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2388,7 +2816,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809535007"/>
@@ -2467,7 +2895,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="sv-SE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2505,7 +2933,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="sv-SE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="809536447"/>
@@ -2547,7 +2975,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="sv-SE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2577,7 +3005,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="sv-SE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4261,15 +4689,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>454397</xdr:colOff>
+      <xdr:colOff>693882</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>89366</xdr:rowOff>
+      <xdr:rowOff>45823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>473447</xdr:colOff>
+      <xdr:colOff>712932</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>103654</xdr:rowOff>
+      <xdr:rowOff>60111</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4298,14 +4726,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>364994</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>28686</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>50458</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>426944</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>88446</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4332,16 +4760,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>754874</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>34762</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>743988</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>45648</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>791934</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>106136</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4370,9 +4798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4410,7 +4838,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4516,7 +4944,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4658,7 +5086,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4666,18 +5094,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F866C2-EAE0-4C7D-BC8B-3898A897A04C}">
-  <dimension ref="A1:Y33"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4700,8 +5129,11 @@
       <c r="W1" t="s">
         <v>7</v>
       </c>
+      <c r="AA1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4762,8 +5194,23 @@
       <c r="Y2" t="s">
         <v>4</v>
       </c>
+      <c r="AA2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:31">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4777,7 +5224,7 @@
       <c r="E3">
         <v>0.50929999999999997</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>20.694050000000001</v>
       </c>
       <c r="H3">
@@ -4828,13 +5275,31 @@
       <c r="Y3">
         <v>15.22405</v>
       </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <f>128*128/AA3</f>
+        <v>16384</v>
+      </c>
+      <c r="AC3">
+        <v>5.4293000000000001E-2</v>
+      </c>
+      <c r="AD3">
+        <f>0.292029</f>
+        <v>0.29202899999999998</v>
+      </c>
+      <c r="AE3">
+        <f>13.23403</f>
+        <v>13.234030000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:31">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C9" si="0">1/(A4*C$1/$B$14)</f>
+        <f t="shared" ref="C4:C8" si="0">1/(A4*C$1/$B$14)</f>
         <v>192</v>
       </c>
       <c r="D4">
@@ -4843,7 +5308,7 @@
       <c r="E4">
         <v>0.53956999999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>21.31138</v>
       </c>
       <c r="H4">
@@ -4894,8 +5359,24 @@
       <c r="Y4">
         <v>15.190060000000001</v>
       </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" ref="AB4:AB16" si="4">128*128/AA4</f>
+        <v>8192</v>
+      </c>
+      <c r="AC4">
+        <v>4.5301000000000001E-2</v>
+      </c>
+      <c r="AD4">
+        <v>0.30060100000000001</v>
+      </c>
+      <c r="AE4">
+        <v>14.017124000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:31">
       <c r="A5">
         <v>8</v>
       </c>
@@ -4960,8 +5441,25 @@
       <c r="Y5">
         <v>23.212949999999999</v>
       </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="4"/>
+        <v>4096</v>
+      </c>
+      <c r="AC5">
+        <v>3.7762999999999998E-2</v>
+      </c>
+      <c r="AD5">
+        <v>0.30715399999999998</v>
+      </c>
+      <c r="AE5">
+        <f>14.83764</f>
+        <v>14.83764</v>
+      </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:31">
       <c r="A6">
         <v>16</v>
       </c>
@@ -5013,8 +5511,25 @@
       <c r="Y6">
         <v>25.822620000000001</v>
       </c>
+      <c r="AA6">
+        <v>8</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="4"/>
+        <v>2048</v>
+      </c>
+      <c r="AC6">
+        <v>3.1025E-2</v>
+      </c>
+      <c r="AD6">
+        <v>0.31353500000000001</v>
+      </c>
+      <c r="AE6">
+        <f>15.698761</f>
+        <v>15.698760999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:31">
       <c r="A7">
         <v>32</v>
       </c>
@@ -5066,8 +5581,25 @@
       <c r="Y7">
         <v>27.599319999999999</v>
       </c>
+      <c r="AA7">
+        <v>16</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="AC7">
+        <v>2.4815E-2</v>
+      </c>
+      <c r="AD7">
+        <v>0.32470500000000002</v>
+      </c>
+      <c r="AE7">
+        <f>16.671994</f>
+        <v>16.671994000000002</v>
+      </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:31">
       <c r="A8">
         <v>64</v>
       </c>
@@ -5106,8 +5638,24 @@
       <c r="Y8">
         <v>32.474519999999998</v>
       </c>
+      <c r="AA8">
+        <v>32</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="AC8">
+        <v>1.9449999999999999E-2</v>
+      </c>
+      <c r="AD8">
+        <v>0.34683000000000003</v>
+      </c>
+      <c r="AE8">
+        <v>17.749154999999998</v>
+      </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:31">
       <c r="W9">
         <v>16</v>
       </c>
@@ -5117,8 +5665,24 @@
       <c r="Y9">
         <v>35.93103</v>
       </c>
+      <c r="AA9">
+        <v>64</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="AC9">
+        <v>1.4952999999999999E-2</v>
+      </c>
+      <c r="AD9">
+        <v>0.38312200000000002</v>
+      </c>
+      <c r="AE9">
+        <v>18.925094999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:31">
       <c r="W10">
         <v>12</v>
       </c>
@@ -5128,8 +5692,24 @@
       <c r="Y10">
         <v>38.738869999999999</v>
       </c>
+      <c r="AA10">
+        <v>128</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="AC10">
+        <v>1.1183999999999999E-2</v>
+      </c>
+      <c r="AD10">
+        <v>0.43704999999999999</v>
+      </c>
+      <c r="AE10">
+        <v>20.223462999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:31">
       <c r="W11">
         <v>6</v>
       </c>
@@ -5139,8 +5719,24 @@
       <c r="Y11">
         <v>46.776229999999998</v>
       </c>
+      <c r="AA11">
+        <v>256</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="AC11">
+        <v>8.1150000000000007E-3</v>
+      </c>
+      <c r="AD11">
+        <v>0.50856400000000002</v>
+      </c>
+      <c r="AE11">
+        <v>21.655605999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:31">
       <c r="W12">
         <v>4</v>
       </c>
@@ -5150,8 +5746,24 @@
       <c r="Y12">
         <v>50.997239999999998</v>
       </c>
+      <c r="AA12">
+        <v>512</v>
+      </c>
+      <c r="AB12" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="AC12">
+        <v>5.6670000000000002E-3</v>
+      </c>
+      <c r="AD12">
+        <v>0.59536900000000004</v>
+      </c>
+      <c r="AE12">
+        <v>23.256789999999999</v>
+      </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:31">
       <c r="W13">
         <v>3</v>
       </c>
@@ -5161,8 +5773,24 @@
       <c r="Y13">
         <v>52.296109999999999</v>
       </c>
+      <c r="AA13">
+        <v>1024</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="AC13">
+        <v>3.7680000000000001E-3</v>
+      </c>
+      <c r="AD13">
+        <v>0.68652500000000005</v>
+      </c>
+      <c r="AE13">
+        <v>25.073186</v>
+      </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -5179,9 +5807,61 @@
       <c r="Y14">
         <v>52.420479999999998</v>
       </c>
+      <c r="AA14">
+        <v>2048</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AC14">
+        <v>2.3210000000000001E-3</v>
+      </c>
+      <c r="AD14">
+        <v>0.77143700000000004</v>
+      </c>
+      <c r="AE14">
+        <v>27.225166999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
+      <c r="AA15">
+        <v>4096</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AC15">
+        <v>1.2570000000000001E-3</v>
+      </c>
+      <c r="AD15">
+        <v>0.84755199999999997</v>
+      </c>
+      <c r="AE15">
+        <v>29.940572</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="AA16">
+        <v>8192</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="AC16">
+        <v>5.13E-4</v>
+      </c>
+      <c r="AD16">
+        <v>0.91810999999999998</v>
+      </c>
+      <c r="AE16">
+        <v>33.897015000000003</v>
+      </c>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="2"/>
+      <c r="E33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>